<commit_message>
Finish Parameter Tab feature. Working on Info and Player Tab
</commit_message>
<xml_diff>
--- a/Tennis_Web/wwwroot/Files/Giai_Dau.xlsx
+++ b/Tennis_Web/wwwroot/Files/Giai_Dau.xlsx
@@ -12,13 +12,12 @@
     <sheet state="visible" name="DS_VDV" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="DS_Vong" sheetId="8" r:id="rId11"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Id</t>
   </si>
@@ -155,13 +154,13 @@
   </numFmts>
   <fonts count="3">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -179,60 +178,28 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -430,17 +397,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="4" width="9.14"/>
-    <col customWidth="1" min="5" max="26" width="8.71"/>
+    <col min="1" max="4" width="9.14" customWidth="1"/>
+    <col min="5" max="26" width="8.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1463,22 +1431,23 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="7" width="9.14"/>
-    <col customWidth="1" min="8" max="26" width="8.71"/>
+    <col min="1" max="7" width="9.14" customWidth="1"/>
+    <col min="8" max="26" width="8.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2507,22 +2476,23 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="5" width="9.14"/>
-    <col customWidth="1" min="6" max="26" width="8.71"/>
+    <col min="1" max="5" width="9.14" customWidth="1"/>
+    <col min="6" max="26" width="8.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3547,22 +3517,23 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="4" width="9.14"/>
-    <col customWidth="1" min="5" max="26" width="8.71"/>
+    <col min="1" max="4" width="9.14" customWidth="1"/>
+    <col min="5" max="26" width="8.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3603,7 +3574,7 @@
     </row>
     <row r="2">
       <c r="C2" s="2">
-        <v>44470.0</v>
+        <v>44470</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>12</v>
@@ -4593,23 +4564,24 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="6" width="9.14"/>
-    <col customWidth="1" min="7" max="7" width="9.29"/>
-    <col customWidth="1" min="8" max="26" width="8.71"/>
+    <col min="1" max="6" width="9.14" customWidth="1"/>
+    <col min="7" max="7" width="9.29" customWidth="1"/>
+    <col min="8" max="26" width="8.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5638,33 +5610,34 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.14"/>
-    <col customWidth="1" min="2" max="2" width="11.0"/>
-    <col customWidth="1" min="3" max="3" width="9.14"/>
-    <col customWidth="1" min="4" max="4" width="9.43"/>
-    <col customWidth="1" min="5" max="5" width="9.14"/>
-    <col customWidth="1" min="6" max="6" width="10.71"/>
-    <col customWidth="1" min="7" max="7" width="9.14"/>
-    <col customWidth="1" min="8" max="8" width="13.0"/>
-    <col customWidth="1" min="9" max="9" width="9.57"/>
-    <col customWidth="1" min="10" max="10" width="10.71"/>
-    <col customWidth="1" min="11" max="11" width="10.43"/>
-    <col customWidth="1" min="12" max="12" width="9.14"/>
-    <col customWidth="1" min="13" max="26" width="8.71"/>
+    <col min="1" max="1" width="9.14" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="9.14" customWidth="1"/>
+    <col min="4" max="4" width="9.43" customWidth="1"/>
+    <col min="5" max="5" width="9.14" customWidth="1"/>
+    <col min="6" max="6" width="10.71" customWidth="1"/>
+    <col min="7" max="7" width="9.14" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="9.57" customWidth="1"/>
+    <col min="10" max="10" width="10.71" customWidth="1"/>
+    <col min="11" max="11" width="10.43" customWidth="1"/>
+    <col min="12" max="12" width="9.14" customWidth="1"/>
+    <col min="13" max="26" width="8.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5721,18 +5694,39 @@
     </row>
     <row r="2">
       <c r="A2" s="3">
-        <v>2.0</v>
+        <v>2</v>
+      </c>
+      <c r="C2" s="0">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0">
+        <v>8</v>
+      </c>
+      <c r="G2" s="0">
+        <v>66</v>
+      </c>
+      <c r="H2" s="0">
+        <v>9</v>
+      </c>
+      <c r="I2" s="0">
+        <v>7</v>
+      </c>
+      <c r="J2" s="0">
+        <v>10</v>
       </c>
       <c r="L2" s="3">
-        <v>1350.0</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="L3" s="3">
-        <v>1280.0</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -6719,25 +6713,26 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="9" width="9.14"/>
-    <col customWidth="1" min="10" max="10" width="11.0"/>
-    <col customWidth="1" min="11" max="11" width="10.29"/>
-    <col customWidth="1" min="12" max="15" width="9.14"/>
-    <col customWidth="1" min="16" max="26" width="8.71"/>
+    <col min="1" max="9" width="9.14" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="10.29" customWidth="1"/>
+    <col min="12" max="15" width="9.14" customWidth="1"/>
+    <col min="16" max="26" width="8.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -7782,22 +7777,23 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="3" width="9.14"/>
-    <col customWidth="1" min="4" max="26" width="8.71"/>
+    <col min="1" max="3" width="9.14" customWidth="1"/>
+    <col min="4" max="26" width="8.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -8818,6 +8814,6 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>